<commit_message>
Switched default curve interpolation to date based
</commit_message>
<xml_diff>
--- a/ExcelExamples/FitCurveNelsonSiegel.xlsx
+++ b/ExcelExamples/FitCurveNelsonSiegel.xlsx
@@ -9,13 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -36,6 +35,9 @@
   </si>
   <si>
     <t>curveName</t>
+  </si>
+  <si>
+    <t>anchorDate</t>
   </si>
 </sst>
 </file>
@@ -112,7 +114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -120,6 +122,7 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,6 +164,433 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-ZA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>data</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>42619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43348</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43713</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44443</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44808</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45173</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45538</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46268</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46633</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47363</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47728</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48093</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>48458</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48823</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>49188</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49553</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>49918</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6.5736587667399995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5830307067000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9929401341100006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0809355823199994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0052032233599996E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8542585422599995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6763059717200002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4964999132500001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3270287282600002E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.1729575038099999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.0355764682699995E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.9142913264800002E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.8076679419299999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.7139916198900002E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6315516600799998E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.5587734439299994E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.4942683142499999E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4368410854899999E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3854773603699996E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.3393226715299997E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.2976596996600007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>fitted</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>42619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43348</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43713</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44078</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44443</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44808</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45173</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45538</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46268</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>46633</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47363</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47728</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48093</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>48458</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48823</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>49188</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49553</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>49918</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$5:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>7.0115188343339352E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4270982512689154E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.671827624400529E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7914588227298992E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8215128414933083E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7886115593107874E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.7125998856556882E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.608174206509688E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.4861303643460539E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3543186673757699E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.2183734984682335E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.082269677451894E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.948745806359935E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.8196256082648829E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6960611461658381E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.5787163057170778E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.4679046776561916E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.3636926984335665E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.2659763806452828E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.17453801797452E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.0890877504997408E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="348273280"/>
+        <c:axId val="348271360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="348273280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="348271360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="348271360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="348273280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F27"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +892,7 @@
     <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -484,13 +914,13 @@
         <v>6</v>
       </c>
       <c r="F3" s="2" t="str">
-        <f ca="1">C27</f>
-        <v>nsCurve1.09:08:40-2</v>
+        <f>C28</f>
+        <v>nsCurve1.12:38:39-15</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>0.05</v>
+      <c r="B4" s="7">
+        <v>42619</v>
       </c>
       <c r="C4" s="4">
         <v>6.5736587667399995E-2</v>
@@ -500,329 +930,318 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>1.05</v>
+      <c r="B5" s="7">
+        <v>42983</v>
       </c>
       <c r="C5" s="4">
         <v>7.5830307067000002E-2</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.05</v>
+      <c r="E5" s="7">
+        <v>42619</v>
       </c>
       <c r="F5" s="6">
-        <f t="array" aca="1" ref="F5:F25" ca="1">_xll.QSA.CurveInterp(C27,B4:B24)</f>
-        <v>6.5736587667399884E-2</v>
+        <f t="array" ref="F5:F25">_xll.QSA.CurveInterp(C28,B4:B24)</f>
+        <v>7.0115188343339352E-2</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>2.0499999999999998</v>
+      <c r="B6" s="7">
+        <v>43348</v>
       </c>
       <c r="C6" s="4">
         <v>7.9929401341100006E-2</v>
       </c>
-      <c r="E6" s="2">
-        <v>1.05</v>
+      <c r="E6" s="7">
+        <v>42983</v>
       </c>
       <c r="F6" s="6">
-        <f ca="1"/>
-        <v>7.5830307067000613E-2</v>
+        <v>7.4270982512689154E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>3.05</v>
+      <c r="B7" s="7">
+        <v>43713</v>
       </c>
       <c r="C7" s="4">
         <v>8.0809355823199994E-2</v>
       </c>
-      <c r="E7" s="2">
-        <v>2.0499999999999998</v>
+      <c r="E7" s="7">
+        <v>43348</v>
       </c>
       <c r="F7" s="6">
-        <f ca="1"/>
-        <v>7.9929401341103282E-2</v>
+        <v>7.671827624400529E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>4.05</v>
+      <c r="B8" s="7">
+        <v>44078</v>
       </c>
       <c r="C8" s="4">
         <v>8.0052032233599996E-2</v>
       </c>
-      <c r="E8" s="2">
-        <v>3.05</v>
+      <c r="E8" s="7">
+        <v>43713</v>
       </c>
       <c r="F8" s="6">
-        <f ca="1"/>
-        <v>8.0809355823205239E-2</v>
+        <v>7.7914588227298992E-2</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>5.05</v>
+      <c r="B9" s="7">
+        <v>44443</v>
       </c>
       <c r="C9" s="4">
         <v>7.8542585422599995E-2</v>
       </c>
-      <c r="E9" s="2">
-        <v>4.05</v>
+      <c r="E9" s="7">
+        <v>44078</v>
       </c>
       <c r="F9" s="6">
-        <f ca="1"/>
-        <v>8.0052032233611486E-2</v>
+        <v>7.8215128414933083E-2</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>6.05</v>
+      <c r="B10" s="7">
+        <v>44808</v>
       </c>
       <c r="C10" s="4">
         <v>7.6763059717200002E-2</v>
       </c>
-      <c r="E10" s="2">
-        <v>5.05</v>
+      <c r="E10" s="7">
+        <v>44443</v>
       </c>
       <c r="F10" s="6">
-        <f ca="1"/>
-        <v>7.8542585422564787E-2</v>
+        <v>7.7886115593107874E-2</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>7.05</v>
+      <c r="B11" s="7">
+        <v>45173</v>
       </c>
       <c r="C11" s="4">
         <v>7.4964999132500001E-2</v>
       </c>
-      <c r="E11" s="2">
-        <v>6.05</v>
+      <c r="E11" s="7">
+        <v>44808</v>
       </c>
       <c r="F11" s="6">
-        <f ca="1"/>
-        <v>7.6763059717173121E-2</v>
+        <v>7.7125998856556882E-2</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>8.0500000000000007</v>
+      <c r="B12" s="7">
+        <v>45538</v>
       </c>
       <c r="C12" s="4">
         <v>7.3270287282600002E-2</v>
       </c>
-      <c r="E12" s="2">
-        <v>7.05</v>
+      <c r="E12" s="7">
+        <v>45173</v>
       </c>
       <c r="F12" s="6">
-        <f ca="1"/>
-        <v>7.4964999132518945E-2</v>
+        <v>7.608174206509688E-2</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>9.0500000000000007</v>
+      <c r="B13" s="7">
+        <v>45903</v>
       </c>
       <c r="C13" s="4">
         <v>7.1729575038099999E-2</v>
       </c>
-      <c r="E13" s="2">
-        <v>8.0500000000000007</v>
+      <c r="E13" s="7">
+        <v>45538</v>
       </c>
       <c r="F13" s="6">
-        <f ca="1"/>
-        <v>7.3270287282617821E-2</v>
+        <v>7.4861303643460539E-2</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>10.050000000000001</v>
+      <c r="B14" s="7">
+        <v>46268</v>
       </c>
       <c r="C14" s="4">
         <v>7.0355764682699995E-2</v>
       </c>
-      <c r="E14" s="2">
-        <v>9.0500000000000007</v>
+      <c r="E14" s="7">
+        <v>45903</v>
       </c>
       <c r="F14" s="6">
-        <f ca="1"/>
-        <v>7.1729575038089716E-2</v>
+        <v>7.3543186673757699E-2</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>11.05</v>
+      <c r="B15" s="7">
+        <v>46633</v>
       </c>
       <c r="C15" s="4">
         <v>6.9142913264800002E-2</v>
       </c>
-      <c r="E15" s="2">
-        <v>10.050000000000001</v>
+      <c r="E15" s="7">
+        <v>46268</v>
       </c>
       <c r="F15" s="6">
-        <f ca="1"/>
-        <v>7.0355764682754299E-2</v>
+        <v>7.2183734984682335E-2</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>12.05</v>
+      <c r="B16" s="7">
+        <v>46998</v>
       </c>
       <c r="C16" s="4">
         <v>6.8076679419299999E-2</v>
       </c>
-      <c r="E16" s="2">
-        <v>11.05</v>
+      <c r="E16" s="7">
+        <v>46633</v>
       </c>
       <c r="F16" s="6">
-        <f ca="1"/>
-        <v>6.9142913264794492E-2</v>
+        <v>7.082269677451894E-2</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>13.05</v>
+      <c r="B17" s="7">
+        <v>47363</v>
       </c>
       <c r="C17" s="4">
         <v>6.7139916198900002E-2</v>
       </c>
-      <c r="E17" s="2">
-        <v>12.05</v>
+      <c r="E17" s="7">
+        <v>46998</v>
       </c>
       <c r="F17" s="6">
-        <f ca="1"/>
-        <v>6.8076679419274602E-2</v>
+        <v>6.948745806359935E-2</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <v>14.05</v>
+      <c r="B18" s="7">
+        <v>47728</v>
       </c>
       <c r="C18" s="4">
         <v>6.6315516600799998E-2</v>
       </c>
-      <c r="E18" s="2">
-        <v>13.05</v>
+      <c r="E18" s="7">
+        <v>47363</v>
       </c>
       <c r="F18" s="6">
-        <f ca="1"/>
-        <v>6.7139916198910826E-2</v>
+        <v>6.8196256082648829E-2</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>15.05</v>
+      <c r="B19" s="7">
+        <v>48093</v>
       </c>
       <c r="C19" s="4">
         <v>6.5587734439299994E-2</v>
       </c>
-      <c r="E19" s="2">
-        <v>14.05</v>
+      <c r="E19" s="7">
+        <v>47728</v>
       </c>
       <c r="F19" s="6">
-        <f ca="1"/>
-        <v>6.6315516600818192E-2</v>
+        <v>6.6960611461658381E-2</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <v>16.05</v>
+      <c r="B20" s="7">
+        <v>48458</v>
       </c>
       <c r="C20" s="4">
         <v>6.4942683142499999E-2</v>
       </c>
-      <c r="E20" s="2">
-        <v>15.05</v>
+      <c r="E20" s="7">
+        <v>48093</v>
       </c>
       <c r="F20" s="6">
-        <f ca="1"/>
-        <v>6.5587734439275486E-2</v>
+        <v>6.5787163057170778E-2</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <v>17.05</v>
+      <c r="B21" s="7">
+        <v>48823</v>
       </c>
       <c r="C21" s="4">
         <v>6.4368410854899999E-2</v>
       </c>
-      <c r="E21" s="2">
-        <v>16.05</v>
+      <c r="E21" s="7">
+        <v>48458</v>
       </c>
       <c r="F21" s="6">
-        <f ca="1"/>
-        <v>6.4942683142473992E-2</v>
+        <v>6.4679046776561916E-2</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <v>18.05</v>
+      <c r="B22" s="7">
+        <v>49188</v>
       </c>
       <c r="C22" s="4">
         <v>6.3854773603699996E-2</v>
       </c>
-      <c r="E22" s="2">
-        <v>17.05</v>
+      <c r="E22" s="7">
+        <v>48823</v>
       </c>
       <c r="F22" s="6">
-        <f ca="1"/>
-        <v>6.436841085487835E-2</v>
+        <v>6.3636926984335665E-2</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
-        <v>19.05</v>
+      <c r="B23" s="7">
+        <v>49553</v>
       </c>
       <c r="C23" s="4">
         <v>6.3393226715299997E-2</v>
       </c>
-      <c r="E23" s="2">
-        <v>18.05</v>
+      <c r="E23" s="7">
+        <v>49188</v>
       </c>
       <c r="F23" s="6">
-        <f ca="1"/>
-        <v>6.385477360371826E-2</v>
+        <v>6.2659763806452828E-2</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
-        <v>20.05</v>
+      <c r="B24" s="7">
+        <v>49918</v>
       </c>
       <c r="C24" s="4">
         <v>6.2976596996600007E-2</v>
       </c>
-      <c r="E24" s="2">
-        <v>19.05</v>
+      <c r="E24" s="7">
+        <v>49553</v>
       </c>
       <c r="F24" s="6">
-        <f ca="1"/>
-        <v>6.3393226715334247E-2</v>
+        <v>6.17453801797452E-2</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="2">
-        <v>20.05</v>
+      <c r="E25" s="7">
+        <v>49918</v>
       </c>
       <c r="F25" s="6">
-        <f ca="1"/>
-        <v>6.2976596996582174E-2</v>
+        <v>6.0890877504997408E-2</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7">
+        <v>42618</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="3" t="str">
-        <f ca="1">_xll.QSA.FitCurveNelsonSiegel(C26,B4:B24,C4:C24)</f>
-        <v>nsCurve1.09:08:40-2</v>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="str">
+        <f>_xll.QSA.FitCurveNelsonSiegel(C27,C26,B4:B24,C4:C24)</f>
+        <v>nsCurve1.12:38:39-15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved example sheet formatting
</commit_message>
<xml_diff>
--- a/ExcelExamples/FitCurveNelsonSiegel.xlsx
+++ b/ExcelExamples/FitCurveNelsonSiegel.xlsx
@@ -96,7 +96,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,11 +118,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,11 +506,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348273280"/>
-        <c:axId val="348271360"/>
+        <c:axId val="338164736"/>
+        <c:axId val="338494208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="348273280"/>
+        <c:axId val="338164736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,12 +520,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="348271360"/>
+        <c:crossAx val="338494208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="348271360"/>
+        <c:axId val="338494208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="348273280"/>
+        <c:crossAx val="338164736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -883,23 +883,23 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="2" width="38.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -915,14 +915,14 @@
       </c>
       <c r="F3" s="2" t="str">
         <f>C28</f>
-        <v>nsCurve1.12:38:39-15</v>
+        <v>nsCurve1.05:43:10-2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>42619</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>6.5736587667399995E-2</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -930,291 +930,291 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>42983</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>7.5830307067000002E-2</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>42619</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <f t="array" ref="F5:F25">_xll.QSA.CurveInterp(C28,B4:B24)</f>
         <v>7.0115188343339352E-2</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>43348</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>7.9929401341100006E-2</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>42983</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <v>7.4270982512689154E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>43713</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>8.0809355823199994E-2</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>43348</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="7">
         <v>7.671827624400529E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>44078</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>8.0052032233599996E-2</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>43713</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <v>7.7914588227298992E-2</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>44443</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>7.8542585422599995E-2</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>44078</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="7">
         <v>7.8215128414933083E-2</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>44808</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>7.6763059717200002E-2</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>44443</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="7">
         <v>7.7886115593107874E-2</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>45173</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>7.4964999132500001E-2</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>44808</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="7">
         <v>7.7125998856556882E-2</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>45538</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>7.3270287282600002E-2</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>45173</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="7">
         <v>7.608174206509688E-2</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>45903</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>7.1729575038099999E-2</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>45538</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="7">
         <v>7.4861303643460539E-2</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>46268</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>7.0355764682699995E-2</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>45903</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="7">
         <v>7.3543186673757699E-2</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>46633</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>6.9142913264800002E-2</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>46268</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="7">
         <v>7.2183734984682335E-2</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>46998</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>6.8076679419299999E-2</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <v>46633</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="7">
         <v>7.082269677451894E-2</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>47363</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>6.7139916198900002E-2</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>46998</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="7">
         <v>6.948745806359935E-2</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>47728</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>6.6315516600799998E-2</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>47363</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="7">
         <v>6.8196256082648829E-2</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>48093</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>6.5587734439299994E-2</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>47728</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="7">
         <v>6.6960611461658381E-2</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>48458</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>6.4942683142499999E-2</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>48093</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="7">
         <v>6.5787163057170778E-2</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>48823</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>6.4368410854899999E-2</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <v>48458</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="7">
         <v>6.4679046776561916E-2</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>49188</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>6.3854773603699996E-2</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <v>48823</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="7">
         <v>6.3636926984335665E-2</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>49553</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>6.3393226715299997E-2</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <v>49188</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="7">
         <v>6.2659763806452828E-2</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>49918</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>6.2976596996600007E-2</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>49553</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="7">
         <v>6.17453801797452E-2</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>49918</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="7">
         <v>6.0890877504997408E-2</v>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <v>42618</v>
       </c>
     </row>
@@ -1235,9 +1235,9 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="3" t="str">
+      <c r="C28" s="6" t="str">
         <f>_xll.QSA.FitCurveNelsonSiegel(C27,C26,B4:B24,C4:C24)</f>
-        <v>nsCurve1.12:38:39-15</v>
+        <v>nsCurve1.05:43:10-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>